<commit_message>
optimized experience type = long -> int
</commit_message>
<xml_diff>
--- a/utilities/AutoSave/data/quests.xlsx
+++ b/utilities/AutoSave/data/quests.xlsx
@@ -39,12 +39,6 @@
     <t>giveGold</t>
   </si>
   <si>
-    <t>npcKillAmountNeeded</t>
-  </si>
-  <si>
-    <t>userKillAmountNeeded</t>
-  </si>
-  <si>
     <t>giveDiamonds</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>Player3</t>
+  </si>
+  <si>
+    <t>npcAmountNeed</t>
+  </si>
+  <si>
+    <t>userAmountNeed</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,8 @@
     <col min="1" max="1" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
@@ -497,10 +498,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -509,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
@@ -522,10 +523,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -586,10 +587,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7">
         <v>8</v>
@@ -619,10 +620,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>10</v>
@@ -652,10 +653,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="7">
         <v>12</v>
@@ -685,10 +686,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7">
         <v>14</v>
@@ -718,10 +719,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7">
         <v>16</v>
@@ -751,10 +752,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="7">
         <v>18</v>
@@ -784,10 +785,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="7">
         <v>20</v>
@@ -817,10 +818,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="7">
         <v>25</v>
@@ -850,10 +851,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="7">
         <v>0</v>
@@ -881,10 +882,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
@@ -912,10 +913,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="7">
         <v>0</v>

</xml_diff>